<commit_message>
Uniformly formatted all the files
</commit_message>
<xml_diff>
--- a/README.xlsx
+++ b/README.xlsx
@@ -613,13 +613,13 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="8"/>
-    <col min="2" max="2" width="34.77734375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="40.77734375" style="8" customWidth="1"/>
     <col min="3" max="3" width="12" style="8" customWidth="1"/>
     <col min="4" max="4" width="42.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5546875" style="8" customWidth="1"/>
@@ -743,7 +743,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>